<commit_message>
Fixes #1 (again :)
</commit_message>
<xml_diff>
--- a/00-仕様書/機能仕様書.xlsx
+++ b/00-仕様書/機能仕様書.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>L</t>
     <phoneticPr fontId="1"/>
@@ -654,6 +654,39 @@
     </rPh>
     <rPh sb="43" eb="46">
       <t>サイサクセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Note:</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/KentVu/kanji-decomposition/issues?state=open</t>
+  </si>
+  <si>
+    <t>これからの要望機能などはGitHubページで登録、閲覧機能がありますので、このページをご参照ください。</t>
+    <rPh sb="5" eb="7">
+      <t>ヨウボウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>エツラン</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>サンショウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1473,7 +1506,7 @@
   <dimension ref="F5:DH71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="CC50" sqref="CC50"/>
+      <selection activeCell="CD57" sqref="CD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -4574,12 +4607,24 @@
       <c r="BW55" s="15"/>
       <c r="BX55" s="15"/>
       <c r="BY55" s="16"/>
+      <c r="CC55" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="CD55" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="56" spans="7:82" ht="19.2" x14ac:dyDescent="0.2">
       <c r="AN56" s="27"/>
+      <c r="CD56" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="57" spans="7:82" ht="19.2" x14ac:dyDescent="0.2">
       <c r="AN57" s="27"/>
+      <c r="CD57" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="58" spans="7:82" ht="19.2" x14ac:dyDescent="0.2">
       <c r="AN58" s="27"/>

</xml_diff>

<commit_message>
Working on #5, 50% completed
</commit_message>
<xml_diff>
--- a/00-仕様書/機能仕様書.xlsx
+++ b/00-仕様書/機能仕様書.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>L</t>
     <phoneticPr fontId="1"/>
@@ -658,37 +658,23 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>*</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Note:</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://github.com/KentVu/kanji-decomposition/issues?state=open</t>
-  </si>
-  <si>
-    <t>これからの要望機能などはGitHubページで登録、閲覧機能がありますので、このページをご参照ください。</t>
-    <rPh sb="5" eb="7">
-      <t>ヨウボウ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>キノウ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
+    <t>これから期待するものはGitHubで表示、登録ができるので、ご利用ください</t>
+    <rPh sb="4" eb="6">
+      <t>キタイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
       <t>トウロク</t>
     </rPh>
-    <rPh sb="25" eb="27">
-      <t>エツラン</t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t>キノウ</t>
-    </rPh>
-    <rPh sb="44" eb="46">
-      <t>サンショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
+    <rPh sb="31" eb="33">
+      <t>リヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/KentVu/kanji-decomposition/issues?state=closed</t>
   </si>
 </sst>
 </file>
@@ -1505,7 +1491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F5:DH71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="CD57" sqref="CD57"/>
     </sheetView>
   </sheetViews>
@@ -4607,23 +4593,17 @@
       <c r="BW55" s="15"/>
       <c r="BX55" s="15"/>
       <c r="BY55" s="16"/>
-      <c r="CC55" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="CD55" s="1" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="56" spans="7:82" ht="19.2" x14ac:dyDescent="0.2">
       <c r="AN56" s="27"/>
       <c r="CD56" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="7:82" ht="19.2" x14ac:dyDescent="0.2">
       <c r="AN57" s="27"/>
       <c r="CD57" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="7:82" ht="19.2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
#5 now supported, closes #5
</commit_message>
<xml_diff>
--- a/00-仕様書/機能仕様書.xlsx
+++ b/00-仕様書/機能仕様書.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LSI\Documents\GitHub\kanji-decomposition\00-仕様書\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16296" windowHeight="5280"/>
   </bookViews>
   <sheets>
     <sheet name="仕様書" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +24,7 @@
     <author>LSI</author>
   </authors>
   <commentList>
-    <comment ref="CC40" authorId="0" shapeId="0">
+    <comment ref="CC40" authorId="0">
       <text>
         <r>
           <rPr>
@@ -674,14 +669,15 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>https://github.com/KentVu/kanji-decomposition/issues?state=closed</t>
+    <t>https://github.com/KentVu/kanji-decomposition/issues</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -773,6 +769,14 @@
       <color theme="0" tint="-0.249977111117893"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -1047,12 +1051,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1197,6 +1204,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1210,7 +1220,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1269,7 +1280,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1304,7 +1315,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1481,7 +1492,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1492,7 +1503,7 @@
   <dimension ref="F5:DH71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="CD57" sqref="CD57"/>
+      <selection activeCell="CJ52" sqref="CJ52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1628,10 +1639,10 @@
       <c r="AA8" s="12"/>
       <c r="AB8" s="13"/>
       <c r="AC8" s="6"/>
-      <c r="AD8" s="48" t="s">
+      <c r="AD8" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="AE8" s="49"/>
+      <c r="AE8" s="50"/>
       <c r="AF8" s="7"/>
       <c r="AG8" s="6"/>
       <c r="AH8" s="6"/>
@@ -1662,10 +1673,10 @@
       <c r="BE8" s="12"/>
       <c r="BF8" s="13"/>
       <c r="BG8" s="6"/>
-      <c r="BH8" s="48" t="s">
+      <c r="BH8" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="BI8" s="49"/>
+      <c r="BI8" s="50"/>
       <c r="BJ8" s="7"/>
     </row>
     <row r="9" spans="7:62" x14ac:dyDescent="0.2">
@@ -1692,8 +1703,8 @@
       <c r="AA9" s="15"/>
       <c r="AB9" s="16"/>
       <c r="AC9" s="6"/>
-      <c r="AD9" s="50"/>
-      <c r="AE9" s="51"/>
+      <c r="AD9" s="51"/>
+      <c r="AE9" s="52"/>
       <c r="AF9" s="7"/>
       <c r="AG9" s="6"/>
       <c r="AH9" s="6"/>
@@ -1722,8 +1733,8 @@
       <c r="BE9" s="15"/>
       <c r="BF9" s="16"/>
       <c r="BG9" s="6"/>
-      <c r="BH9" s="50"/>
-      <c r="BI9" s="51"/>
+      <c r="BH9" s="51"/>
+      <c r="BI9" s="52"/>
       <c r="BJ9" s="7"/>
     </row>
     <row r="10" spans="7:62" x14ac:dyDescent="0.2">
@@ -4602,7 +4613,7 @@
     </row>
     <row r="57" spans="7:82" ht="19.2" x14ac:dyDescent="0.2">
       <c r="AN57" s="27"/>
-      <c r="CD57" s="1" t="s">
+      <c r="CD57" s="48" t="s">
         <v>50</v>
       </c>
     </row>
@@ -4666,8 +4677,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="CD57" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>